<commit_message>
modification .gitignore et modifications/ménage dossiers
</commit_message>
<xml_diff>
--- a/readme_pages/step_1__location_cases.xlsx
+++ b/readme_pages/step_1__location_cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_portfolio\Job_Market\readme_pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFDA4B9-BA2F-469C-802F-0018CDE9EBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9C7128-D74F-4F6F-8F3F-1455379C68BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62F386FC-F515-440B-9A20-824FDE3DF32B}"/>
   </bookViews>
@@ -183,13 +183,6 @@
 _region</t>
   </si>
   <si>
-    <t>répartition sur le fichier archivé 
-"_offres_concatenated_13639_offres__2025-03-05--22h09.json"</t>
-  </si>
-  <si>
-    <t>attributs conservés</t>
-  </si>
-  <si>
     <t>code
 _postal</t>
   </si>
@@ -207,10 +200,17 @@
     <t>Après (récupération des données de localisation)</t>
   </si>
   <si>
-    <t>Données récupérées à partir du fichier "codes__city_department_region.csv"</t>
-  </si>
-  <si>
     <t>Avant (données disponibles de base)</t>
+  </si>
+  <si>
+    <t>attributs à conserver</t>
+  </si>
+  <si>
+    <t>Données récupérées à partir du fichier "code_name__city_department_region.csv"</t>
+  </si>
+  <si>
+    <t>répartition sur le fichier archivé 
+"2025-03-12--21h13__2__with_location_attributes.json"</t>
   </si>
 </sst>
 </file>
@@ -835,12 +835,12 @@
   <dimension ref="B3:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.36328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
@@ -850,23 +850,23 @@
     <col min="9" max="9" width="1.08984375" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.81640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="1.08984375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.453125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.08984375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.54296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.08984375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5.453125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.08984375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.54296875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.81640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.1796875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="1" customWidth="1"/>
     <col min="20" max="20" width="0.453125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -875,7 +875,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="L4" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -888,7 +888,7 @@
     <row r="5" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="2:21" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D6" s="21" t="s">
@@ -899,7 +899,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="23"/>
       <c r="L6" s="26" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="M6" s="26"/>
       <c r="N6" s="26"/>
@@ -935,16 +935,16 @@
         <v>15</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>43</v>
@@ -959,7 +959,7 @@
         <v>46</v>
       </c>
       <c r="U7" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -987,17 +987,17 @@
       <c r="J8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="19">
         <v>75012</v>
       </c>
       <c r="M8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="5">
+        <v>75012</v>
+      </c>
+      <c r="O8" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="N8" s="19">
-        <v>75012</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>5</v>
       </c>
       <c r="P8" s="14">
         <v>75</v>
@@ -1040,14 +1040,14 @@
       <c r="J9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="14">
-        <v>59800</v>
+      <c r="L9" s="15">
+        <v>59350</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="15">
-        <v>59350</v>
+      <c r="N9" s="14">
+        <v>59800</v>
       </c>
       <c r="O9" s="14" t="s">
         <v>21</v>
@@ -1230,7 +1230,7 @@
     <row r="13" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="2:21" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D14" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
@@ -1252,7 +1252,7 @@
     <row r="17" spans="19:19" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="19:19" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S18" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="19:19" ht="18.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>